<commit_message>
country added to data scraped
</commit_message>
<xml_diff>
--- a/webcrawler/Scraped Data.xlsx
+++ b/webcrawler/Scraped Data.xlsx
@@ -13,10 +13,13 @@
   </bookViews>
   <sheets>
     <sheet name="Scraped Data" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Scraped Data'!$G$1:$G$102</definedName>
-    <definedName name="scrapeddata" localSheetId="0">'Scraped Data'!$B$2:$F$102</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Scraped Data'!$H$1:$H$102</definedName>
+    <definedName name="scrapeddata" localSheetId="0">'Scraped Data'!$B$2:$G$102</definedName>
+    <definedName name="scrp2" localSheetId="0">'Scraped Data'!$C$2:$C$102</definedName>
+    <definedName name="scrp2" localSheetId="1">Sheet1!$A$1:$A$101</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -37,11 +40,39 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="2" name="scrp2" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr sourceFile="D:\Programs\Jetbrains\327\nsu.spring2019.cse327.1.t4\webcrawler\scrp2.csv" delimiter="|">
+      <textFields count="8">
+        <textField type="skip"/>
+        <textField/>
+        <textField type="skip"/>
+        <textField type="skip"/>
+        <textField type="skip"/>
+        <textField type="skip"/>
+        <textField type="skip"/>
+        <textField type="skip"/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="3" name="scrp21" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr sourceFile="D:\Programs\Jetbrains\327\nsu.spring2019.cse327.1.t4\webcrawler\scrp2.csv" delimiter="|">
+      <textFields count="8">
+        <textField type="skip"/>
+        <textField/>
+        <textField type="skip"/>
+        <textField type="skip"/>
+        <textField type="skip"/>
+        <textField type="skip"/>
+        <textField type="skip"/>
+        <textField type="skip"/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="245">
   <si>
     <t xml:space="preserve">Massachusetts Institute of Technology (MIT) </t>
   </si>
@@ -707,6 +738,75 @@
   </si>
   <si>
     <t>Scholarships</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> United States </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> United Kingdom </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Switzerland </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Singapore </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> China </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Japan </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Australia </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hong Kong </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Canada </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> South Korea </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> France </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Netherlands </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Germany </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Taiwan </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Argentina </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Denmark </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Belgium </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> New Zealand </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Malaysia </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Russia </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sweden </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Leeds </t>
   </si>
 </sst>
 </file>
@@ -1252,7 +1352,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="scrp2" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="scrapeddata" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="scrp2" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1518,23 +1626,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H102"/>
+  <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.140625" customWidth="1"/>
     <col min="2" max="2" width="53.5703125" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" customWidth="1"/>
-    <col min="4" max="5" width="10.42578125" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" customWidth="1"/>
+    <col min="5" max="6" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>214</v>
       </c>
@@ -1542,25 +1651,28 @@
         <v>215</v>
       </c>
       <c r="C1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D1" t="s">
         <v>216</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>217</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>218</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>219</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>220</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1568,19 +1680,22 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="1">
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1">
         <v>11145</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1588,39 +1703,45 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
+        <v>223</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="1">
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="1">
         <v>16135</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C4" t="s">
+        <v>223</v>
+      </c>
+      <c r="E4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="1">
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="1">
         <v>22727</v>
       </c>
-      <c r="G4" s="1">
+      <c r="H4" s="1">
         <v>4542</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1628,19 +1749,22 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
+        <v>223</v>
+      </c>
+      <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>3</v>
       </c>
-      <c r="E5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="1">
+      <c r="F5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="1">
         <v>2239</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1648,39 +1772,45 @@
         <v>13</v>
       </c>
       <c r="C6" t="s">
+        <v>224</v>
+      </c>
+      <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
       <c r="E6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="1">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="1">
         <v>20631</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
       </c>
-      <c r="D7" t="s">
-        <v>16</v>
+      <c r="C7" t="s">
+        <v>224</v>
       </c>
       <c r="E7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="1">
+        <v>16</v>
+      </c>
+      <c r="F7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="1">
         <v>19203</v>
       </c>
-      <c r="G7" s="1">
+      <c r="H7" s="1">
         <v>5601</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1688,19 +1818,22 @@
         <v>19</v>
       </c>
       <c r="C8" t="s">
+        <v>225</v>
+      </c>
+      <c r="D8" t="s">
         <v>21</v>
       </c>
-      <c r="D8" t="s">
-        <v>16</v>
-      </c>
       <c r="E8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" s="1">
+        <v>16</v>
+      </c>
+      <c r="F8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="1">
         <v>18003</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1708,19 +1841,22 @@
         <v>22</v>
       </c>
       <c r="C9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D9" t="s">
         <v>15</v>
       </c>
-      <c r="D9" t="s">
-        <v>16</v>
-      </c>
       <c r="E9" t="s">
-        <v>4</v>
-      </c>
-      <c r="F9" s="1">
+        <v>16</v>
+      </c>
+      <c r="F9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="1">
         <v>16797</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -1728,19 +1864,22 @@
         <v>24</v>
       </c>
       <c r="C10" t="s">
+        <v>223</v>
+      </c>
+      <c r="D10" t="s">
         <v>26</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>3</v>
       </c>
-      <c r="E10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F10" s="1">
+      <c r="F10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="1">
         <v>13924</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -1748,79 +1887,91 @@
         <v>27</v>
       </c>
       <c r="C11" t="s">
+        <v>224</v>
+      </c>
+      <c r="D11" t="s">
         <v>15</v>
       </c>
-      <c r="D11" t="s">
-        <v>16</v>
-      </c>
       <c r="E11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" s="1">
+        <v>16</v>
+      </c>
+      <c r="F11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="1">
         <v>32795</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
       <c r="B12" t="s">
         <v>29</v>
       </c>
-      <c r="D12" t="s">
-        <v>16</v>
+      <c r="C12" t="s">
+        <v>226</v>
       </c>
       <c r="E12" t="s">
-        <v>4</v>
-      </c>
-      <c r="F12" s="1">
+        <v>16</v>
+      </c>
+      <c r="F12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="1">
         <v>30226</v>
       </c>
-      <c r="G12" s="1">
+      <c r="H12" s="1">
         <v>4766</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>32</v>
       </c>
       <c r="B13" t="s">
         <v>31</v>
       </c>
-      <c r="D13" t="s">
-        <v>16</v>
+      <c r="C13" t="s">
+        <v>226</v>
       </c>
       <c r="E13" t="s">
-        <v>4</v>
-      </c>
-      <c r="F13" s="1">
+        <v>16</v>
+      </c>
+      <c r="F13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="1">
         <v>25088</v>
       </c>
-      <c r="G13" s="1">
+      <c r="H13" s="1">
         <v>4216</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>34</v>
       </c>
       <c r="B14" t="s">
         <v>33</v>
       </c>
-      <c r="D14" t="s">
+      <c r="C14" t="s">
+        <v>223</v>
+      </c>
+      <c r="E14" t="s">
         <v>3</v>
       </c>
-      <c r="E14" t="s">
-        <v>4</v>
-      </c>
-      <c r="F14" s="1">
+      <c r="F14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="1">
         <v>8017</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>987</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -1828,19 +1979,22 @@
         <v>35</v>
       </c>
       <c r="C15" t="s">
+        <v>223</v>
+      </c>
+      <c r="D15" t="s">
         <v>26</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>3</v>
       </c>
-      <c r="E15" t="s">
-        <v>4</v>
-      </c>
-      <c r="F15" s="1">
+      <c r="F15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="1">
         <v>22144</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -1848,59 +2002,68 @@
         <v>37</v>
       </c>
       <c r="C16" t="s">
+        <v>223</v>
+      </c>
+      <c r="D16" t="s">
         <v>26</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>3</v>
       </c>
-      <c r="E16" t="s">
-        <v>4</v>
-      </c>
-      <c r="F16" s="1">
+      <c r="F16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" s="1">
         <v>12927</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>40</v>
       </c>
       <c r="B17" t="s">
         <v>39</v>
       </c>
-      <c r="D17" t="s">
+      <c r="C17" t="s">
+        <v>223</v>
+      </c>
+      <c r="E17" t="s">
         <v>3</v>
       </c>
-      <c r="E17" t="s">
-        <v>4</v>
-      </c>
-      <c r="F17" s="1">
+      <c r="F17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="1">
         <v>26160</v>
       </c>
-      <c r="G17" s="1">
+      <c r="H17" s="1">
         <v>6315</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>42</v>
       </c>
       <c r="B18" t="s">
         <v>41</v>
       </c>
-      <c r="D18" t="s">
-        <v>16</v>
+      <c r="C18" t="s">
+        <v>227</v>
       </c>
       <c r="E18" t="s">
-        <v>4</v>
-      </c>
-      <c r="F18" s="1">
+        <v>16</v>
+      </c>
+      <c r="F18" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" s="1">
         <v>36403</v>
       </c>
-      <c r="G18" s="1">
+      <c r="H18" s="1">
         <v>5716</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>44</v>
       </c>
@@ -1908,19 +2071,22 @@
         <v>43</v>
       </c>
       <c r="C19" t="s">
+        <v>224</v>
+      </c>
+      <c r="D19" t="s">
         <v>45</v>
       </c>
-      <c r="D19" t="s">
-        <v>16</v>
-      </c>
       <c r="E19" t="s">
-        <v>4</v>
-      </c>
-      <c r="F19" s="1">
+        <v>16</v>
+      </c>
+      <c r="F19" t="s">
+        <v>4</v>
+      </c>
+      <c r="G19" s="1">
         <v>29222</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -1928,19 +2094,22 @@
         <v>46</v>
       </c>
       <c r="C20" t="s">
+        <v>223</v>
+      </c>
+      <c r="D20" t="s">
         <v>48</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>3</v>
       </c>
-      <c r="E20" t="s">
-        <v>4</v>
-      </c>
-      <c r="F20" s="1">
+      <c r="F20" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="1">
         <v>20852</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -1948,19 +2117,22 @@
         <v>49</v>
       </c>
       <c r="C21" t="s">
+        <v>223</v>
+      </c>
+      <c r="D21" t="s">
         <v>51</v>
       </c>
-      <c r="D21" t="s">
-        <v>16</v>
-      </c>
       <c r="E21" t="s">
-        <v>4</v>
-      </c>
-      <c r="F21" s="1">
+        <v>16</v>
+      </c>
+      <c r="F21" t="s">
+        <v>4</v>
+      </c>
+      <c r="G21" s="1">
         <v>43874</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -1968,19 +2140,22 @@
         <v>52</v>
       </c>
       <c r="C22" t="s">
+        <v>223</v>
+      </c>
+      <c r="D22" t="s">
         <v>26</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>3</v>
       </c>
-      <c r="E22" t="s">
-        <v>4</v>
-      </c>
-      <c r="F22" s="1">
+      <c r="F22" t="s">
+        <v>4</v>
+      </c>
+      <c r="G22" s="1">
         <v>16657</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>55</v>
       </c>
@@ -1988,39 +2163,45 @@
         <v>54</v>
       </c>
       <c r="C23" t="s">
+        <v>225</v>
+      </c>
+      <c r="D23" t="s">
         <v>21</v>
       </c>
-      <c r="D23" t="s">
-        <v>16</v>
-      </c>
       <c r="E23" t="s">
-        <v>4</v>
-      </c>
-      <c r="F23" s="1">
+        <v>16</v>
+      </c>
+      <c r="F23" t="s">
+        <v>4</v>
+      </c>
+      <c r="G23" s="1">
         <v>10492</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>57</v>
       </c>
       <c r="B24" t="s">
         <v>56</v>
       </c>
-      <c r="D24" t="s">
-        <v>16</v>
+      <c r="C24" t="s">
+        <v>228</v>
       </c>
       <c r="E24" t="s">
-        <v>4</v>
-      </c>
-      <c r="F24" s="1">
+        <v>16</v>
+      </c>
+      <c r="F24" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24" s="1">
         <v>27407</v>
       </c>
-      <c r="G24" s="1">
+      <c r="H24" s="1">
         <v>4522</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>59</v>
       </c>
@@ -2028,59 +2209,68 @@
         <v>58</v>
       </c>
       <c r="C25" t="s">
+        <v>229</v>
+      </c>
+      <c r="D25" t="s">
         <v>51</v>
       </c>
-      <c r="D25" t="s">
-        <v>16</v>
-      </c>
       <c r="E25" t="s">
-        <v>4</v>
-      </c>
-      <c r="F25" s="1">
+        <v>16</v>
+      </c>
+      <c r="F25" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25" s="1">
         <v>16677</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>61</v>
       </c>
       <c r="B26" t="s">
         <v>60</v>
       </c>
-      <c r="D26" t="s">
-        <v>16</v>
+      <c r="C26" t="s">
+        <v>230</v>
       </c>
       <c r="E26" t="s">
-        <v>4</v>
-      </c>
-      <c r="F26" s="1">
+        <v>16</v>
+      </c>
+      <c r="F26" t="s">
+        <v>4</v>
+      </c>
+      <c r="G26" s="1">
         <v>20203</v>
       </c>
-      <c r="G26" s="1">
+      <c r="H26" s="1">
         <v>3013</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>63</v>
       </c>
       <c r="B27" t="s">
         <v>62</v>
       </c>
-      <c r="D27" t="s">
+      <c r="C27" t="s">
+        <v>223</v>
+      </c>
+      <c r="E27" t="s">
         <v>3</v>
       </c>
-      <c r="E27" t="s">
-        <v>4</v>
-      </c>
-      <c r="F27" s="1">
+      <c r="F27" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" s="1">
         <v>15086</v>
       </c>
-      <c r="G27" s="1">
+      <c r="H27" s="1">
         <v>3037</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>65</v>
       </c>
@@ -2088,19 +2278,22 @@
         <v>64</v>
       </c>
       <c r="C28" t="s">
+        <v>223</v>
+      </c>
+      <c r="D28" t="s">
         <v>51</v>
       </c>
-      <c r="D28" t="s">
-        <v>16</v>
-      </c>
       <c r="E28" t="s">
-        <v>4</v>
-      </c>
-      <c r="F28" s="1">
+        <v>16</v>
+      </c>
+      <c r="F28" t="s">
+        <v>4</v>
+      </c>
+      <c r="G28" s="1">
         <v>40056</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>67</v>
       </c>
@@ -2108,19 +2301,22 @@
         <v>66</v>
       </c>
       <c r="C29" t="s">
+        <v>231</v>
+      </c>
+      <c r="D29" t="s">
         <v>68</v>
       </c>
-      <c r="D29" t="s">
-        <v>16</v>
-      </c>
       <c r="E29" t="s">
-        <v>4</v>
-      </c>
-      <c r="F29" s="1">
+        <v>16</v>
+      </c>
+      <c r="F29" t="s">
+        <v>4</v>
+      </c>
+      <c r="G29" s="1">
         <v>73064</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>70</v>
       </c>
@@ -2128,59 +2324,68 @@
         <v>69</v>
       </c>
       <c r="C30" t="s">
+        <v>224</v>
+      </c>
+      <c r="D30" t="s">
         <v>71</v>
       </c>
-      <c r="D30" t="s">
-        <v>16</v>
-      </c>
       <c r="E30" t="s">
-        <v>4</v>
-      </c>
-      <c r="F30" s="1">
+        <v>16</v>
+      </c>
+      <c r="F30" t="s">
+        <v>4</v>
+      </c>
+      <c r="G30" s="1">
         <v>37577</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>73</v>
       </c>
       <c r="B31" t="s">
         <v>72</v>
       </c>
-      <c r="D31" t="s">
-        <v>16</v>
+      <c r="C31" t="s">
+        <v>227</v>
       </c>
       <c r="E31" t="s">
-        <v>4</v>
-      </c>
-      <c r="F31" s="1">
+        <v>16</v>
+      </c>
+      <c r="F31" t="s">
+        <v>4</v>
+      </c>
+      <c r="G31" s="1">
         <v>43242</v>
       </c>
-      <c r="G31" s="1">
+      <c r="H31" s="1">
         <v>5019</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>75</v>
       </c>
       <c r="B32" t="s">
         <v>74</v>
       </c>
-      <c r="D32" t="s">
-        <v>16</v>
+      <c r="C32" t="s">
+        <v>224</v>
       </c>
       <c r="E32" t="s">
-        <v>4</v>
-      </c>
-      <c r="F32" s="1">
+        <v>16</v>
+      </c>
+      <c r="F32" t="s">
+        <v>4</v>
+      </c>
+      <c r="G32" s="1">
         <v>25977</v>
       </c>
-      <c r="G32" s="1">
+      <c r="H32" s="1">
         <v>3730</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>77</v>
       </c>
@@ -2188,19 +2393,22 @@
         <v>76</v>
       </c>
       <c r="C33" t="s">
+        <v>223</v>
+      </c>
+      <c r="D33" t="s">
         <v>71</v>
       </c>
-      <c r="D33" t="s">
-        <v>16</v>
-      </c>
       <c r="E33" t="s">
-        <v>4</v>
-      </c>
-      <c r="F33" s="1">
+        <v>16</v>
+      </c>
+      <c r="F33" t="s">
+        <v>4</v>
+      </c>
+      <c r="G33" s="1">
         <v>43800</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>79</v>
       </c>
@@ -2208,19 +2416,22 @@
         <v>78</v>
       </c>
       <c r="C34" t="s">
+        <v>231</v>
+      </c>
+      <c r="D34" t="s">
         <v>68</v>
       </c>
-      <c r="D34" t="s">
-        <v>16</v>
-      </c>
       <c r="E34" t="s">
-        <v>4</v>
-      </c>
-      <c r="F34" s="1">
+        <v>16</v>
+      </c>
+      <c r="F34" t="s">
+        <v>4</v>
+      </c>
+      <c r="G34" s="1">
         <v>29102</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>81</v>
       </c>
@@ -2228,159 +2439,183 @@
         <v>80</v>
       </c>
       <c r="C35" t="s">
+        <v>223</v>
+      </c>
+      <c r="D35" t="s">
         <v>26</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>3</v>
       </c>
-      <c r="E35" t="s">
-        <v>4</v>
-      </c>
-      <c r="F35" s="1">
+      <c r="F35" t="s">
+        <v>4</v>
+      </c>
+      <c r="G35" s="1">
         <v>18924</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>83</v>
       </c>
       <c r="B36" t="s">
         <v>82</v>
       </c>
-      <c r="D36" t="s">
-        <v>16</v>
+      <c r="C36" t="s">
+        <v>228</v>
       </c>
       <c r="E36" t="s">
-        <v>4</v>
-      </c>
-      <c r="F36" s="1">
+        <v>16</v>
+      </c>
+      <c r="F36" t="s">
+        <v>4</v>
+      </c>
+      <c r="G36" s="1">
         <v>23081</v>
       </c>
-      <c r="G36" s="1">
+      <c r="H36" s="1">
         <v>3947</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>85</v>
       </c>
       <c r="B37" t="s">
         <v>84</v>
       </c>
-      <c r="D37" t="s">
-        <v>16</v>
+      <c r="C37" t="s">
+        <v>232</v>
       </c>
       <c r="E37" t="s">
-        <v>4</v>
-      </c>
-      <c r="F37" s="1">
+        <v>16</v>
+      </c>
+      <c r="F37" t="s">
+        <v>4</v>
+      </c>
+      <c r="G37" s="1">
         <v>28482</v>
       </c>
-      <c r="G37" s="1">
+      <c r="H37" s="1">
         <v>4226</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>87</v>
       </c>
       <c r="B38" t="s">
         <v>86</v>
       </c>
-      <c r="D38" t="s">
-        <v>16</v>
+      <c r="C38" t="s">
+        <v>230</v>
       </c>
       <c r="E38" t="s">
-        <v>4</v>
-      </c>
-      <c r="F38" s="1">
+        <v>16</v>
+      </c>
+      <c r="F38" t="s">
+        <v>4</v>
+      </c>
+      <c r="G38" s="1">
         <v>10666</v>
       </c>
-      <c r="G38" s="1">
+      <c r="H38" s="1">
         <v>1213</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>89</v>
       </c>
       <c r="B39" t="s">
         <v>88</v>
       </c>
-      <c r="D39" t="s">
-        <v>16</v>
+      <c r="C39" t="s">
+        <v>224</v>
       </c>
       <c r="E39" t="s">
-        <v>4</v>
-      </c>
-      <c r="F39" s="1">
+        <v>16</v>
+      </c>
+      <c r="F39" t="s">
+        <v>4</v>
+      </c>
+      <c r="G39" s="1">
         <v>10357</v>
       </c>
-      <c r="G39">
+      <c r="H39">
         <v>947</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>91</v>
       </c>
       <c r="B40" t="s">
         <v>90</v>
       </c>
-      <c r="D40" t="s">
-        <v>16</v>
+      <c r="C40" t="s">
+        <v>229</v>
       </c>
       <c r="E40" t="s">
-        <v>4</v>
-      </c>
-      <c r="F40" s="1">
+        <v>16</v>
+      </c>
+      <c r="F40" t="s">
+        <v>4</v>
+      </c>
+      <c r="G40" s="1">
         <v>44365</v>
       </c>
-      <c r="H40" t="s">
+      <c r="I40" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>94</v>
       </c>
       <c r="B41" t="s">
         <v>93</v>
       </c>
-      <c r="D41" t="s">
-        <v>16</v>
+      <c r="C41" t="s">
+        <v>232</v>
       </c>
       <c r="E41" t="s">
-        <v>4</v>
-      </c>
-      <c r="F41" s="1">
+        <v>16</v>
+      </c>
+      <c r="F41" t="s">
+        <v>4</v>
+      </c>
+      <c r="G41" s="1">
         <v>9812</v>
       </c>
-      <c r="G41" s="1">
+      <c r="H41" s="1">
         <v>1323</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>96</v>
       </c>
       <c r="B42" t="s">
         <v>95</v>
       </c>
-      <c r="D42" t="s">
-        <v>16</v>
+      <c r="C42" t="s">
+        <v>223</v>
       </c>
       <c r="E42" t="s">
-        <v>4</v>
-      </c>
-      <c r="F42" s="1">
+        <v>16</v>
+      </c>
+      <c r="F42" t="s">
+        <v>4</v>
+      </c>
+      <c r="G42" s="1">
         <v>33935</v>
       </c>
-      <c r="G42" s="1">
+      <c r="H42" s="1">
         <v>3868</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>98</v>
       </c>
@@ -2388,19 +2623,22 @@
         <v>97</v>
       </c>
       <c r="C43" t="s">
+        <v>229</v>
+      </c>
+      <c r="D43" t="s">
         <v>99</v>
       </c>
-      <c r="D43" t="s">
-        <v>16</v>
-      </c>
       <c r="E43" t="s">
-        <v>4</v>
-      </c>
-      <c r="F43" s="1">
+        <v>16</v>
+      </c>
+      <c r="F43" t="s">
+        <v>4</v>
+      </c>
+      <c r="G43" s="1">
         <v>44817</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>101</v>
       </c>
@@ -2408,39 +2646,45 @@
         <v>100</v>
       </c>
       <c r="C44" t="s">
+        <v>223</v>
+      </c>
+      <c r="D44" t="s">
         <v>2</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
         <v>3</v>
       </c>
-      <c r="E44" t="s">
-        <v>4</v>
-      </c>
-      <c r="F44" s="1">
+      <c r="F44" t="s">
+        <v>4</v>
+      </c>
+      <c r="G44" s="1">
         <v>44433</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>103</v>
       </c>
       <c r="B45" t="s">
         <v>102</v>
       </c>
-      <c r="D45" t="s">
-        <v>16</v>
+      <c r="C45" t="s">
+        <v>227</v>
       </c>
       <c r="E45" t="s">
-        <v>4</v>
-      </c>
-      <c r="F45" s="1">
+        <v>16</v>
+      </c>
+      <c r="F45" t="s">
+        <v>4</v>
+      </c>
+      <c r="G45" s="1">
         <v>31354</v>
       </c>
-      <c r="G45" s="1">
+      <c r="H45" s="1">
         <v>4481</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>105</v>
       </c>
@@ -2448,19 +2692,22 @@
         <v>104</v>
       </c>
       <c r="C46" t="s">
+        <v>229</v>
+      </c>
+      <c r="D46" t="s">
         <v>106</v>
       </c>
-      <c r="D46" t="s">
-        <v>16</v>
-      </c>
       <c r="E46" t="s">
-        <v>4</v>
-      </c>
-      <c r="F46" s="1">
+        <v>16</v>
+      </c>
+      <c r="F46" t="s">
+        <v>4</v>
+      </c>
+      <c r="G46" s="1">
         <v>40326</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>108</v>
       </c>
@@ -2468,19 +2715,22 @@
         <v>107</v>
       </c>
       <c r="C47" t="s">
+        <v>223</v>
+      </c>
+      <c r="D47" t="s">
         <v>109</v>
       </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
         <v>3</v>
       </c>
-      <c r="E47" t="s">
-        <v>4</v>
-      </c>
-      <c r="F47" s="1">
+      <c r="F47" t="s">
+        <v>4</v>
+      </c>
+      <c r="G47" s="1">
         <v>13991</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>111</v>
       </c>
@@ -2488,19 +2738,22 @@
         <v>110</v>
       </c>
       <c r="C48" t="s">
+        <v>231</v>
+      </c>
+      <c r="D48" t="s">
         <v>45</v>
       </c>
-      <c r="D48" t="s">
-        <v>16</v>
-      </c>
       <c r="E48" t="s">
-        <v>4</v>
-      </c>
-      <c r="F48" s="1">
+        <v>16</v>
+      </c>
+      <c r="F48" t="s">
+        <v>4</v>
+      </c>
+      <c r="G48" s="1">
         <v>52970</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>113</v>
       </c>
@@ -2508,39 +2761,45 @@
         <v>112</v>
       </c>
       <c r="C49" t="s">
+        <v>229</v>
+      </c>
+      <c r="D49" t="s">
         <v>106</v>
       </c>
-      <c r="D49" t="s">
-        <v>16</v>
-      </c>
       <c r="E49" t="s">
-        <v>4</v>
-      </c>
-      <c r="F49" s="1">
+        <v>16</v>
+      </c>
+      <c r="F49" t="s">
+        <v>4</v>
+      </c>
+      <c r="G49" s="1">
         <v>39436</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>115</v>
       </c>
       <c r="B50" t="s">
         <v>114</v>
       </c>
-      <c r="D50" t="s">
-        <v>16</v>
+      <c r="C50" t="s">
+        <v>230</v>
       </c>
       <c r="E50" t="s">
-        <v>4</v>
-      </c>
-      <c r="F50" s="1">
+        <v>16</v>
+      </c>
+      <c r="F50" t="s">
+        <v>4</v>
+      </c>
+      <c r="G50" s="1">
         <v>17705</v>
       </c>
-      <c r="G50" s="1">
+      <c r="H50" s="1">
         <v>2300</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>117</v>
       </c>
@@ -2548,19 +2807,22 @@
         <v>116</v>
       </c>
       <c r="C51" t="s">
+        <v>233</v>
+      </c>
+      <c r="D51" t="s">
         <v>45</v>
       </c>
-      <c r="D51" t="s">
-        <v>16</v>
-      </c>
       <c r="E51" t="s">
-        <v>4</v>
-      </c>
-      <c r="F51" s="1">
+        <v>16</v>
+      </c>
+      <c r="F51" t="s">
+        <v>4</v>
+      </c>
+      <c r="G51" s="1">
         <v>20234</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>119</v>
       </c>
@@ -2568,19 +2830,22 @@
         <v>118</v>
       </c>
       <c r="C52" t="s">
+        <v>224</v>
+      </c>
+      <c r="D52" t="s">
         <v>15</v>
       </c>
-      <c r="D52" t="s">
-        <v>16</v>
-      </c>
       <c r="E52" t="s">
-        <v>4</v>
-      </c>
-      <c r="F52" s="1">
+        <v>16</v>
+      </c>
+      <c r="F52" t="s">
+        <v>4</v>
+      </c>
+      <c r="G52" s="1">
         <v>21906</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>121</v>
       </c>
@@ -2588,19 +2853,22 @@
         <v>120</v>
       </c>
       <c r="C53" t="s">
+        <v>234</v>
+      </c>
+      <c r="D53" t="s">
         <v>45</v>
       </c>
-      <c r="D53" t="s">
-        <v>16</v>
-      </c>
       <c r="E53" t="s">
-        <v>4</v>
-      </c>
-      <c r="F53" s="1">
+        <v>16</v>
+      </c>
+      <c r="F53" t="s">
+        <v>4</v>
+      </c>
+      <c r="G53" s="1">
         <v>17703</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>123</v>
       </c>
@@ -2608,19 +2876,22 @@
         <v>122</v>
       </c>
       <c r="C54" t="s">
+        <v>223</v>
+      </c>
+      <c r="D54" t="s">
         <v>124</v>
       </c>
-      <c r="D54" t="s">
-        <v>16</v>
-      </c>
       <c r="E54" t="s">
-        <v>4</v>
-      </c>
-      <c r="F54" s="1">
+        <v>16</v>
+      </c>
+      <c r="F54" t="s">
+        <v>4</v>
+      </c>
+      <c r="G54" s="1">
         <v>39282</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>126</v>
       </c>
@@ -2628,39 +2899,45 @@
         <v>125</v>
       </c>
       <c r="C55" t="s">
+        <v>224</v>
+      </c>
+      <c r="D55" t="s">
         <v>15</v>
       </c>
-      <c r="D55" t="s">
-        <v>16</v>
-      </c>
       <c r="E55" t="s">
-        <v>4</v>
-      </c>
-      <c r="F55" s="1">
+        <v>16</v>
+      </c>
+      <c r="F55" t="s">
+        <v>4</v>
+      </c>
+      <c r="G55" s="1">
         <v>20884</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>128</v>
       </c>
       <c r="B56" t="s">
         <v>127</v>
       </c>
-      <c r="D56" t="s">
-        <v>16</v>
+      <c r="C56" t="s">
+        <v>230</v>
       </c>
       <c r="E56" t="s">
-        <v>4</v>
-      </c>
-      <c r="F56" s="1">
+        <v>16</v>
+      </c>
+      <c r="F56" t="s">
+        <v>4</v>
+      </c>
+      <c r="G56" s="1">
         <v>9566</v>
       </c>
-      <c r="G56" s="1">
+      <c r="H56" s="1">
         <v>1488</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>130</v>
       </c>
@@ -2668,19 +2945,22 @@
         <v>129</v>
       </c>
       <c r="C57" t="s">
+        <v>223</v>
+      </c>
+      <c r="D57" t="s">
         <v>48</v>
       </c>
-      <c r="D57" t="s">
+      <c r="E57" t="s">
         <v>3</v>
       </c>
-      <c r="E57" t="s">
-        <v>4</v>
-      </c>
-      <c r="F57" s="1">
+      <c r="F57" t="s">
+        <v>4</v>
+      </c>
+      <c r="G57" s="1">
         <v>9564</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>132</v>
       </c>
@@ -2688,79 +2968,91 @@
         <v>131</v>
       </c>
       <c r="C58" t="s">
+        <v>234</v>
+      </c>
+      <c r="D58" t="s">
         <v>45</v>
       </c>
-      <c r="D58" t="s">
-        <v>16</v>
-      </c>
       <c r="E58" t="s">
-        <v>4</v>
-      </c>
-      <c r="F58" s="1">
+        <v>16</v>
+      </c>
+      <c r="F58" t="s">
+        <v>4</v>
+      </c>
+      <c r="G58" s="1">
         <v>23962</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>134</v>
       </c>
       <c r="B59" t="s">
         <v>133</v>
       </c>
-      <c r="D59" t="s">
-        <v>16</v>
+      <c r="C59" t="s">
+        <v>228</v>
       </c>
       <c r="E59" t="s">
-        <v>4</v>
-      </c>
-      <c r="F59" s="1">
+        <v>16</v>
+      </c>
+      <c r="F59" t="s">
+        <v>4</v>
+      </c>
+      <c r="G59" s="1">
         <v>9962</v>
       </c>
-      <c r="G59" s="1">
+      <c r="H59" s="1">
         <v>1538</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>136</v>
       </c>
       <c r="B60" t="s">
         <v>135</v>
       </c>
-      <c r="D60" t="s">
-        <v>16</v>
+      <c r="C60" t="s">
+        <v>229</v>
       </c>
       <c r="E60" t="s">
-        <v>4</v>
-      </c>
-      <c r="F60" s="1">
+        <v>16</v>
+      </c>
+      <c r="F60" t="s">
+        <v>4</v>
+      </c>
+      <c r="G60" s="1">
         <v>57764</v>
       </c>
-      <c r="H60" t="s">
+      <c r="I60" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>136</v>
       </c>
       <c r="B61" t="s">
         <v>137</v>
       </c>
-      <c r="D61" t="s">
-        <v>16</v>
+      <c r="C61" t="s">
+        <v>227</v>
       </c>
       <c r="E61" t="s">
-        <v>4</v>
-      </c>
-      <c r="F61" s="1">
+        <v>16</v>
+      </c>
+      <c r="F61" t="s">
+        <v>4</v>
+      </c>
+      <c r="G61" s="1">
         <v>40830</v>
       </c>
-      <c r="G61" s="1">
+      <c r="H61" s="1">
         <v>3702</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>139</v>
       </c>
@@ -2768,19 +3060,22 @@
         <v>138</v>
       </c>
       <c r="C62" t="s">
+        <v>235</v>
+      </c>
+      <c r="D62" t="s">
         <v>21</v>
       </c>
-      <c r="D62" t="s">
-        <v>16</v>
-      </c>
       <c r="E62" t="s">
-        <v>4</v>
-      </c>
-      <c r="F62" s="1">
+        <v>16</v>
+      </c>
+      <c r="F62" t="s">
+        <v>4</v>
+      </c>
+      <c r="G62" s="1">
         <v>39323</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>141</v>
       </c>
@@ -2788,39 +3083,45 @@
         <v>140</v>
       </c>
       <c r="C63" t="s">
+        <v>235</v>
+      </c>
+      <c r="D63" t="s">
         <v>21</v>
       </c>
-      <c r="D63" t="s">
-        <v>16</v>
-      </c>
       <c r="E63" t="s">
-        <v>4</v>
-      </c>
-      <c r="F63" s="1">
+        <v>16</v>
+      </c>
+      <c r="F63" t="s">
+        <v>4</v>
+      </c>
+      <c r="G63" s="1">
         <v>34689</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>143</v>
       </c>
       <c r="B64" t="s">
         <v>142</v>
       </c>
-      <c r="D64" t="s">
-        <v>16</v>
+      <c r="C64" t="s">
+        <v>223</v>
       </c>
       <c r="E64" t="s">
-        <v>4</v>
-      </c>
-      <c r="F64" s="1">
+        <v>16</v>
+      </c>
+      <c r="F64" t="s">
+        <v>4</v>
+      </c>
+      <c r="G64" s="1">
         <v>48485</v>
       </c>
-      <c r="G64" s="1">
+      <c r="H64" s="1">
         <v>2856</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>145</v>
       </c>
@@ -2828,19 +3129,22 @@
         <v>144</v>
       </c>
       <c r="C65" t="s">
+        <v>235</v>
+      </c>
+      <c r="D65" t="s">
         <v>21</v>
       </c>
-      <c r="D65" t="s">
-        <v>16</v>
-      </c>
       <c r="E65" t="s">
-        <v>4</v>
-      </c>
-      <c r="F65" s="1">
+        <v>16</v>
+      </c>
+      <c r="F65" t="s">
+        <v>4</v>
+      </c>
+      <c r="G65" s="1">
         <v>20800</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>147</v>
       </c>
@@ -2848,79 +3152,91 @@
         <v>146</v>
       </c>
       <c r="C66" t="s">
+        <v>233</v>
+      </c>
+      <c r="D66" t="s">
         <v>21</v>
       </c>
-      <c r="D66" t="s">
-        <v>16</v>
-      </c>
       <c r="E66" t="s">
-        <v>4</v>
-      </c>
-      <c r="F66" s="1">
+        <v>16</v>
+      </c>
+      <c r="F66" t="s">
+        <v>4</v>
+      </c>
+      <c r="G66" s="1">
         <v>2908</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>149</v>
       </c>
       <c r="B67" t="s">
         <v>148</v>
       </c>
-      <c r="D67" t="s">
-        <v>16</v>
+      <c r="C67" t="s">
+        <v>223</v>
       </c>
       <c r="E67" t="s">
-        <v>4</v>
-      </c>
-      <c r="F67" s="1">
+        <v>16</v>
+      </c>
+      <c r="F67" t="s">
+        <v>4</v>
+      </c>
+      <c r="G67" s="1">
         <v>52346</v>
       </c>
-      <c r="G67" s="1">
+      <c r="H67" s="1">
         <v>2796</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>151</v>
       </c>
       <c r="B68" t="s">
         <v>150</v>
       </c>
-      <c r="D68" t="s">
-        <v>16</v>
+      <c r="C68" t="s">
+        <v>228</v>
       </c>
       <c r="E68" t="s">
-        <v>4</v>
-      </c>
-      <c r="F68" s="1">
+        <v>16</v>
+      </c>
+      <c r="F68" t="s">
+        <v>4</v>
+      </c>
+      <c r="G68" s="1">
         <v>22520</v>
       </c>
-      <c r="G68" s="1">
+      <c r="H68" s="1">
         <v>3095</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>153</v>
       </c>
       <c r="B69" t="s">
         <v>152</v>
       </c>
-      <c r="D69" t="s">
-        <v>16</v>
+      <c r="C69" t="s">
+        <v>227</v>
       </c>
       <c r="E69" t="s">
-        <v>4</v>
-      </c>
-      <c r="F69" s="1">
+        <v>16</v>
+      </c>
+      <c r="F69" t="s">
+        <v>4</v>
+      </c>
+      <c r="G69" s="1">
         <v>33650</v>
       </c>
-      <c r="G69" s="1">
+      <c r="H69" s="1">
         <v>5408</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>155</v>
       </c>
@@ -2928,19 +3244,22 @@
         <v>154</v>
       </c>
       <c r="C70" t="s">
+        <v>223</v>
+      </c>
+      <c r="D70" t="s">
         <v>156</v>
       </c>
-      <c r="D70" t="s">
-        <v>16</v>
-      </c>
       <c r="E70" t="s">
-        <v>4</v>
-      </c>
-      <c r="F70" s="1">
+        <v>16</v>
+      </c>
+      <c r="F70" t="s">
+        <v>4</v>
+      </c>
+      <c r="G70" s="1">
         <v>22007</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>155</v>
       </c>
@@ -2948,79 +3267,91 @@
         <v>157</v>
       </c>
       <c r="C71" t="s">
+        <v>224</v>
+      </c>
+      <c r="D71" t="s">
         <v>45</v>
       </c>
-      <c r="D71" t="s">
-        <v>16</v>
-      </c>
       <c r="E71" t="s">
-        <v>4</v>
-      </c>
-      <c r="F71" s="1">
+        <v>16</v>
+      </c>
+      <c r="F71" t="s">
+        <v>4</v>
+      </c>
+      <c r="G71" s="1">
         <v>25150</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>159</v>
       </c>
       <c r="B72" t="s">
         <v>158</v>
       </c>
-      <c r="D72" t="s">
-        <v>16</v>
+      <c r="C72" t="s">
+        <v>223</v>
       </c>
       <c r="E72" t="s">
-        <v>4</v>
-      </c>
-      <c r="F72" s="1">
+        <v>16</v>
+      </c>
+      <c r="F72" t="s">
+        <v>4</v>
+      </c>
+      <c r="G72" s="1">
         <v>43283</v>
       </c>
-      <c r="G72" s="1">
+      <c r="H72" s="1">
         <v>2639</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>161</v>
       </c>
       <c r="B73" t="s">
         <v>160</v>
       </c>
-      <c r="D73" t="s">
-        <v>16</v>
+      <c r="C73" t="s">
+        <v>236</v>
       </c>
       <c r="E73" t="s">
-        <v>4</v>
-      </c>
-      <c r="F73" s="1">
+        <v>16</v>
+      </c>
+      <c r="F73" t="s">
+        <v>4</v>
+      </c>
+      <c r="G73" s="1">
         <v>30625</v>
       </c>
-      <c r="G73" s="1">
+      <c r="H73" s="1">
         <v>2804</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>163</v>
       </c>
       <c r="B74" t="s">
         <v>162</v>
       </c>
-      <c r="D74" t="s">
-        <v>16</v>
+      <c r="C74" t="s">
+        <v>237</v>
       </c>
       <c r="E74" t="s">
-        <v>4</v>
-      </c>
-      <c r="F74" s="1">
+        <v>16</v>
+      </c>
+      <c r="F74" t="s">
+        <v>4</v>
+      </c>
+      <c r="G74" s="1">
         <v>122298</v>
       </c>
-      <c r="G74" s="1">
+      <c r="H74" s="1">
         <v>16419</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>165</v>
       </c>
@@ -3028,19 +3359,22 @@
         <v>164</v>
       </c>
       <c r="C75" t="s">
+        <v>224</v>
+      </c>
+      <c r="D75" t="s">
         <v>15</v>
       </c>
-      <c r="D75" t="s">
-        <v>16</v>
-      </c>
       <c r="E75" t="s">
-        <v>4</v>
-      </c>
-      <c r="F75" s="1">
+        <v>16</v>
+      </c>
+      <c r="F75" t="s">
+        <v>4</v>
+      </c>
+      <c r="G75" s="1">
         <v>17259</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>167</v>
       </c>
@@ -3048,19 +3382,22 @@
         <v>166</v>
       </c>
       <c r="C76" t="s">
+        <v>233</v>
+      </c>
+      <c r="D76" t="s">
         <v>21</v>
       </c>
-      <c r="D76" t="s">
-        <v>16</v>
-      </c>
       <c r="E76" t="s">
-        <v>4</v>
-      </c>
-      <c r="F76" s="1">
+        <v>16</v>
+      </c>
+      <c r="F76" t="s">
+        <v>4</v>
+      </c>
+      <c r="G76" s="1">
         <v>41777</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>167</v>
       </c>
@@ -3068,19 +3405,22 @@
         <v>168</v>
       </c>
       <c r="C77" t="s">
+        <v>224</v>
+      </c>
+      <c r="D77" t="s">
         <v>71</v>
       </c>
-      <c r="D77" t="s">
-        <v>16</v>
-      </c>
       <c r="E77" t="s">
-        <v>4</v>
-      </c>
-      <c r="F77" s="1">
+        <v>16</v>
+      </c>
+      <c r="F77" t="s">
+        <v>4</v>
+      </c>
+      <c r="G77" s="1">
         <v>26429</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>170</v>
       </c>
@@ -3088,19 +3428,22 @@
         <v>169</v>
       </c>
       <c r="C78" t="s">
+        <v>228</v>
+      </c>
+      <c r="D78" t="s">
         <v>21</v>
       </c>
-      <c r="D78" t="s">
-        <v>16</v>
-      </c>
       <c r="E78" t="s">
-        <v>4</v>
-      </c>
-      <c r="F78" s="1">
+        <v>16</v>
+      </c>
+      <c r="F78" t="s">
+        <v>4</v>
+      </c>
+      <c r="G78" s="1">
         <v>26472</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>172</v>
       </c>
@@ -3108,19 +3451,22 @@
         <v>171</v>
       </c>
       <c r="C79" t="s">
+        <v>225</v>
+      </c>
+      <c r="D79" t="s">
         <v>71</v>
       </c>
-      <c r="D79" t="s">
-        <v>16</v>
-      </c>
       <c r="E79" t="s">
-        <v>4</v>
-      </c>
-      <c r="F79" s="1">
+        <v>16</v>
+      </c>
+      <c r="F79" t="s">
+        <v>4</v>
+      </c>
+      <c r="G79" s="1">
         <v>29112</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>172</v>
       </c>
@@ -3128,19 +3474,22 @@
         <v>173</v>
       </c>
       <c r="C80" t="s">
+        <v>224</v>
+      </c>
+      <c r="D80" t="s">
         <v>21</v>
       </c>
-      <c r="D80" t="s">
-        <v>16</v>
-      </c>
       <c r="E80" t="s">
-        <v>4</v>
-      </c>
-      <c r="F80" s="1">
+        <v>16</v>
+      </c>
+      <c r="F80" t="s">
+        <v>4</v>
+      </c>
+      <c r="G80" s="1">
         <v>31177</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>175</v>
       </c>
@@ -3148,19 +3497,22 @@
         <v>174</v>
       </c>
       <c r="C81" t="s">
+        <v>238</v>
+      </c>
+      <c r="D81" t="s">
         <v>21</v>
       </c>
-      <c r="D81" t="s">
-        <v>16</v>
-      </c>
       <c r="E81" t="s">
-        <v>4</v>
-      </c>
-      <c r="F81" s="1">
+        <v>16</v>
+      </c>
+      <c r="F81" t="s">
+        <v>4</v>
+      </c>
+      <c r="G81" s="1">
         <v>45422</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>177</v>
       </c>
@@ -3168,39 +3520,45 @@
         <v>176</v>
       </c>
       <c r="C82" t="s">
+        <v>239</v>
+      </c>
+      <c r="D82" t="s">
         <v>71</v>
       </c>
-      <c r="D82" t="s">
-        <v>16</v>
-      </c>
       <c r="E82" t="s">
-        <v>4</v>
-      </c>
-      <c r="F82" s="1">
+        <v>16</v>
+      </c>
+      <c r="F82" t="s">
+        <v>4</v>
+      </c>
+      <c r="G82" s="1">
         <v>29928</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>179</v>
       </c>
       <c r="B83" t="s">
         <v>178</v>
       </c>
-      <c r="D83" t="s">
+      <c r="C83" t="s">
+        <v>224</v>
+      </c>
+      <c r="E83" t="s">
         <v>3</v>
       </c>
-      <c r="E83" t="s">
-        <v>4</v>
-      </c>
-      <c r="F83" s="1">
+      <c r="F83" t="s">
+        <v>4</v>
+      </c>
+      <c r="G83" s="1">
         <v>3114</v>
       </c>
-      <c r="G83">
+      <c r="H83">
         <v>681</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>179</v>
       </c>
@@ -3208,19 +3566,22 @@
         <v>180</v>
       </c>
       <c r="C84" t="s">
+        <v>232</v>
+      </c>
+      <c r="D84" t="s">
         <v>156</v>
       </c>
-      <c r="D84" t="s">
-        <v>16</v>
-      </c>
       <c r="E84" t="s">
-        <v>4</v>
-      </c>
-      <c r="F84" s="1">
+        <v>16</v>
+      </c>
+      <c r="F84" t="s">
+        <v>4</v>
+      </c>
+      <c r="G84" s="1">
         <v>26211</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>182</v>
       </c>
@@ -3228,39 +3589,45 @@
         <v>181</v>
       </c>
       <c r="C85" t="s">
+        <v>223</v>
+      </c>
+      <c r="D85" t="s">
         <v>68</v>
       </c>
-      <c r="D85" t="s">
-        <v>16</v>
-      </c>
       <c r="E85" t="s">
-        <v>4</v>
-      </c>
-      <c r="F85" s="1">
+        <v>16</v>
+      </c>
+      <c r="F85" t="s">
+        <v>4</v>
+      </c>
+      <c r="G85" s="1">
         <v>29981</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>184</v>
       </c>
       <c r="B86" t="s">
         <v>183</v>
       </c>
-      <c r="D86" t="s">
+      <c r="C86" t="s">
+        <v>240</v>
+      </c>
+      <c r="E86" t="s">
         <v>3</v>
       </c>
-      <c r="E86" t="s">
-        <v>4</v>
-      </c>
-      <c r="F86" s="1">
+      <c r="F86" t="s">
+        <v>4</v>
+      </c>
+      <c r="G86" s="1">
         <v>25226</v>
       </c>
-      <c r="G86" s="1">
+      <c r="H86" s="1">
         <v>3700</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>186</v>
       </c>
@@ -3268,39 +3635,45 @@
         <v>185</v>
       </c>
       <c r="C87" t="s">
+        <v>232</v>
+      </c>
+      <c r="D87" t="s">
         <v>187</v>
       </c>
-      <c r="D87" t="s">
+      <c r="E87" t="s">
         <v>3</v>
       </c>
-      <c r="E87" t="s">
-        <v>4</v>
-      </c>
-      <c r="F87" s="1">
+      <c r="F87" t="s">
+        <v>4</v>
+      </c>
+      <c r="G87" s="1">
         <v>6752</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>186</v>
       </c>
       <c r="B88" t="s">
         <v>188</v>
       </c>
-      <c r="D88" t="s">
-        <v>16</v>
+      <c r="C88" t="s">
+        <v>223</v>
       </c>
       <c r="E88" t="s">
-        <v>4</v>
-      </c>
-      <c r="F88" s="1">
+        <v>16</v>
+      </c>
+      <c r="F88" t="s">
+        <v>4</v>
+      </c>
+      <c r="G88" s="1">
         <v>15140</v>
       </c>
-      <c r="G88" s="1">
+      <c r="H88" s="1">
         <v>2464</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>190</v>
       </c>
@@ -3308,79 +3681,91 @@
         <v>189</v>
       </c>
       <c r="C89" t="s">
+        <v>241</v>
+      </c>
+      <c r="D89" t="s">
         <v>71</v>
       </c>
-      <c r="D89" t="s">
-        <v>16</v>
-      </c>
       <c r="E89" t="s">
-        <v>4</v>
-      </c>
-      <c r="F89" s="1">
+        <v>16</v>
+      </c>
+      <c r="F89" t="s">
+        <v>4</v>
+      </c>
+      <c r="G89" s="1">
         <v>43603</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>192</v>
       </c>
       <c r="B90" t="s">
         <v>191</v>
       </c>
-      <c r="D90" t="s">
-        <v>16</v>
+      <c r="C90" t="s">
+        <v>223</v>
       </c>
       <c r="E90" t="s">
-        <v>4</v>
-      </c>
-      <c r="F90" s="1">
+        <v>16</v>
+      </c>
+      <c r="F90" t="s">
+        <v>4</v>
+      </c>
+      <c r="G90" s="1">
         <v>30904</v>
       </c>
-      <c r="G90" s="1">
+      <c r="H90" s="1">
         <v>6536</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>194</v>
       </c>
       <c r="B91" t="s">
         <v>193</v>
       </c>
-      <c r="D91" t="s">
-        <v>16</v>
+      <c r="C91" t="s">
+        <v>242</v>
       </c>
       <c r="E91" t="s">
-        <v>4</v>
-      </c>
-      <c r="F91" s="1">
+        <v>16</v>
+      </c>
+      <c r="F91" t="s">
+        <v>4</v>
+      </c>
+      <c r="G91" s="1">
         <v>18431</v>
       </c>
-      <c r="H91" t="s">
+      <c r="I91" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>196</v>
       </c>
       <c r="B92" t="s">
         <v>195</v>
       </c>
-      <c r="D92" t="s">
-        <v>16</v>
+      <c r="C92" t="s">
+        <v>229</v>
       </c>
       <c r="E92" t="s">
-        <v>4</v>
-      </c>
-      <c r="F92" s="1">
+        <v>16</v>
+      </c>
+      <c r="F92" t="s">
+        <v>4</v>
+      </c>
+      <c r="G92" s="1">
         <v>27786</v>
       </c>
-      <c r="G92" s="1">
+      <c r="H92" s="1">
         <v>3031</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>198</v>
       </c>
@@ -3388,19 +3773,22 @@
         <v>197</v>
       </c>
       <c r="C93" t="s">
+        <v>243</v>
+      </c>
+      <c r="D93" t="s">
         <v>26</v>
       </c>
-      <c r="D93" t="s">
+      <c r="E93" t="s">
         <v>3</v>
       </c>
-      <c r="E93" t="s">
-        <v>4</v>
-      </c>
-      <c r="F93" s="1">
+      <c r="F93" t="s">
+        <v>4</v>
+      </c>
+      <c r="G93" s="1">
         <v>26508</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>198</v>
       </c>
@@ -3408,19 +3796,22 @@
         <v>199</v>
       </c>
       <c r="C94" t="s">
+        <v>223</v>
+      </c>
+      <c r="D94" t="s">
         <v>15</v>
       </c>
-      <c r="D94" t="s">
-        <v>16</v>
-      </c>
       <c r="E94" t="s">
-        <v>4</v>
-      </c>
-      <c r="F94" s="1">
+        <v>16</v>
+      </c>
+      <c r="F94" t="s">
+        <v>4</v>
+      </c>
+      <c r="G94" s="1">
         <v>30842</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>201</v>
       </c>
@@ -3428,59 +3819,68 @@
         <v>200</v>
       </c>
       <c r="C95" t="s">
+        <v>244</v>
+      </c>
+      <c r="D95" t="s">
         <v>202</v>
       </c>
-      <c r="D95" t="s">
-        <v>16</v>
-      </c>
       <c r="E95" t="s">
-        <v>4</v>
-      </c>
-      <c r="F95" s="1">
+        <v>16</v>
+      </c>
+      <c r="F95" t="s">
+        <v>4</v>
+      </c>
+      <c r="G95" s="1">
         <v>45218</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>204</v>
       </c>
       <c r="B96" t="s">
         <v>203</v>
       </c>
-      <c r="D96" t="s">
-        <v>16</v>
+      <c r="C96" t="s">
+        <v>223</v>
       </c>
       <c r="E96" t="s">
-        <v>4</v>
-      </c>
-      <c r="F96" s="1">
+        <v>16</v>
+      </c>
+      <c r="F96" t="s">
+        <v>4</v>
+      </c>
+      <c r="G96" s="1">
         <v>23197</v>
       </c>
-      <c r="H96" t="s">
+      <c r="I96" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>206</v>
       </c>
       <c r="B97" t="s">
         <v>205</v>
       </c>
-      <c r="D97" t="s">
-        <v>16</v>
+      <c r="C97" t="s">
+        <v>224</v>
       </c>
       <c r="E97" t="s">
-        <v>4</v>
-      </c>
-      <c r="F97" s="1">
+        <v>16</v>
+      </c>
+      <c r="F97" t="s">
+        <v>4</v>
+      </c>
+      <c r="G97" s="1">
         <v>16152</v>
       </c>
-      <c r="G97" s="1">
+      <c r="H97" s="1">
         <v>2065</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>208</v>
       </c>
@@ -3488,19 +3888,22 @@
         <v>207</v>
       </c>
       <c r="C98" t="s">
+        <v>224</v>
+      </c>
+      <c r="D98" t="s">
         <v>45</v>
       </c>
-      <c r="D98" t="s">
-        <v>16</v>
-      </c>
       <c r="E98" t="s">
-        <v>4</v>
-      </c>
-      <c r="F98" s="1">
+        <v>16</v>
+      </c>
+      <c r="F98" t="s">
+        <v>4</v>
+      </c>
+      <c r="G98" s="1">
         <v>8535</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>210</v>
       </c>
@@ -3508,39 +3911,45 @@
         <v>209</v>
       </c>
       <c r="C99" t="s">
+        <v>227</v>
+      </c>
+      <c r="D99" t="s">
         <v>71</v>
       </c>
-      <c r="D99" t="s">
-        <v>16</v>
-      </c>
       <c r="E99" t="s">
-        <v>4</v>
-      </c>
-      <c r="F99" s="1">
+        <v>16</v>
+      </c>
+      <c r="F99" t="s">
+        <v>4</v>
+      </c>
+      <c r="G99" s="1">
         <v>37670</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>210</v>
       </c>
       <c r="B100" t="s">
         <v>211</v>
       </c>
-      <c r="D100" t="s">
+      <c r="C100" t="s">
+        <v>234</v>
+      </c>
+      <c r="E100" t="s">
         <v>3</v>
       </c>
-      <c r="E100" t="s">
-        <v>4</v>
-      </c>
-      <c r="F100" s="1">
+      <c r="F100" t="s">
+        <v>4</v>
+      </c>
+      <c r="G100" s="1">
         <v>23142</v>
       </c>
-      <c r="G100" s="1">
+      <c r="H100" s="1">
         <v>3462</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>210</v>
       </c>
@@ -3548,19 +3957,22 @@
         <v>212</v>
       </c>
       <c r="C101" t="s">
+        <v>223</v>
+      </c>
+      <c r="D101" t="s">
         <v>51</v>
       </c>
-      <c r="D101" t="s">
-        <v>16</v>
-      </c>
       <c r="E101" t="s">
-        <v>4</v>
-      </c>
-      <c r="F101" s="1">
+        <v>16</v>
+      </c>
+      <c r="F101" t="s">
+        <v>4</v>
+      </c>
+      <c r="G101" s="1">
         <v>35430</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>210</v>
       </c>
@@ -3568,16 +3980,542 @@
         <v>213</v>
       </c>
       <c r="C102" t="s">
+        <v>232</v>
+      </c>
+      <c r="D102" t="s">
         <v>2</v>
       </c>
-      <c r="D102" t="s">
+      <c r="E102" t="s">
         <v>3</v>
       </c>
-      <c r="E102" t="s">
-        <v>4</v>
-      </c>
-      <c r="F102" s="1">
+      <c r="F102" t="s">
+        <v>4</v>
+      </c>
+      <c r="G102" s="1">
         <v>13474</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A101"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>